<commit_message>
Added folder for java programs
</commit_message>
<xml_diff>
--- a/program_list.xlsx
+++ b/program_list.xlsx
@@ -7,8 +7,8 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="algo_program" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="algo_programs" sheetId="1" r:id="rId1"/>
+    <sheet name="java_programs" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="69">
   <si>
     <t xml:space="preserve">Sr. No. </t>
   </si>
@@ -214,13 +214,22 @@
   </si>
   <si>
     <t>Find element with given rank 'r' - Using a deterministic procedure - Pivot choose wisely</t>
+  </si>
+  <si>
+    <t>KargerMinCut</t>
+  </si>
+  <si>
+    <t>Java</t>
+  </si>
+  <si>
+    <t>Coursera - Stanford - Karger Min Cut Implementation - See description file for details</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -243,16 +252,42 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor theme="8" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor theme="8" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -260,11 +295,51 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -277,6 +352,33 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -693,8 +795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:F179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -1969,12 +2071,77 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="B2:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="94.42578125" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" ht="16.5" thickBot="1">
+      <c r="B2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="16.5" thickTop="1">
+      <c r="B3" s="8">
+        <v>1</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="15.75">
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="13"/>
+    </row>
+    <row r="5" spans="2:6" ht="15.75">
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="10"/>
+    </row>
+    <row r="6" spans="2:6" ht="15.75">
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="13"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Added new C programs
</commit_message>
<xml_diff>
--- a/program_list.xlsx
+++ b/program_list.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="83">
   <si>
     <t xml:space="preserve">Sr. No. </t>
   </si>
@@ -256,6 +256,12 @@
   </si>
   <si>
     <t xml:space="preserve">Maximum product subsequence in an array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">findFirstMinRHS.c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Find the first number aj smaller than ai such that j &gt; i i.e. aj is on the right – For all numbers </t>
   </si>
   <si>
     <t xml:space="preserve">KargerMinCut</t>
@@ -570,8 +576,8 @@
   </sheetPr>
   <dimension ref="B2:F179"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F37" activeCellId="0" sqref="F37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C39" activeCellId="0" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1193,10 +1199,25 @@
       <c r="E37" s="2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F37" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="1" t="n">
         <v>36</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1962,13 +1983,13 @@
         <v>1</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Added and corrected programs
</commit_message>
<xml_diff>
--- a/program_list.xlsx
+++ b/program_list.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="130">
   <si>
     <t xml:space="preserve">Sr. No. </t>
   </si>
@@ -366,7 +366,34 @@
     <t xml:space="preserve">Insert a node into a Red Black Tree</t>
   </si>
   <si>
-    <t xml:space="preserve">Testing Left</t>
+    <t xml:space="preserve">delRBTree.c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delete a node from a RBT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">modAVL.h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code for AVL insert and delete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testing53.c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testing header file for AVL insert and delete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">modRB.h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Header file for Red Black Tree insertion and deletion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testing55.c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testing header file for Red Black Tree insertion and deletion</t>
   </si>
   <si>
     <t xml:space="preserve">KargerMinCut.java</t>
@@ -541,7 +568,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -566,8 +593,12 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -719,8 +750,8 @@
   </sheetPr>
   <dimension ref="B2:G179"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B53" activeCellId="0" sqref="B53"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E39" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G58" activeCellId="0" sqref="G58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1772,32 +1803,107 @@
         <v>9</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="1" t="n">
         <v>52</v>
       </c>
-    </row>
-    <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C54" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="1" t="n">
         <v>53</v>
       </c>
-    </row>
-    <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C55" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="1" t="n">
         <v>54</v>
       </c>
-    </row>
-    <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C56" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="1" t="n">
         <v>55</v>
       </c>
-    </row>
-    <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C57" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="1" t="n">
         <v>56</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2432,89 +2538,89 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="12.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="7" width="14.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="7" width="85.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="8" width="14.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="7" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="7" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="12.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="8" width="31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="8" width="14.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="8" width="85.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="9" width="14.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="8" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="8" width="8.57"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="13" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="13" t="n">
+      <c r="B3" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="C3" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>117</v>
-      </c>
-      <c r="F3" s="15" t="s">
+      <c r="C3" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="F3" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="17" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="17" t="n">
+      <c r="B4" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="C4" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="F4" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="G4" s="20"/>
+      <c r="C4" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="G4" s="21"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="16"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="17"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="20"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="21"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -2541,7 +2647,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="7" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="8" width="8.57"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Modified programs - 52, 55 and 56
</commit_message>
<xml_diff>
--- a/program_list.xlsx
+++ b/program_list.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="134">
   <si>
     <t xml:space="preserve">Sr. No. </t>
   </si>
@@ -394,6 +394,18 @@
   </si>
   <si>
     <t xml:space="preserve">Testing header file for Red Black Tree insertion and deletion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">findRankBBST.c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Find the rank of an element stored in a BBST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">findElRankBBST.c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Find the element with a given rank stored in BBST</t>
   </si>
   <si>
     <t xml:space="preserve">KargerMinCut.java</t>
@@ -750,8 +762,8 @@
   </sheetPr>
   <dimension ref="B2:G179"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E39" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G58" activeCellId="0" sqref="G58"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A61" activeCellId="0" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1823,7 +1835,7 @@
         <v>9</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1903,17 +1915,47 @@
         <v>9</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="1" t="n">
         <v>57</v>
       </c>
-    </row>
-    <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C59" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="1" t="n">
         <v>58</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2573,13 +2615,13 @@
         <v>1</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="F3" s="16" t="s">
         <v>36</v>
@@ -2593,16 +2635,16 @@
         <v>2</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="G4" s="21"/>
     </row>

</xml_diff>